<commit_message>
erd and data update
</commit_message>
<xml_diff>
--- a/Mock UI Forms.xlsx
+++ b/Mock UI Forms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vipe1\Documents\School\CIT 225\sts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3280A474-3441-4C3F-ACB7-D71292FD06A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6176BDFB-1332-4727-A5B8-AB26942219A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="9982" activeTab="3" xr2:uid="{BE137E8C-EC77-4330-B204-71CF6D8543D7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="3" xr2:uid="{BE137E8C-EC77-4330-B204-71CF6D8543D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
   <si>
     <t>What are we creating?</t>
   </si>
@@ -70,13 +70,7 @@
     <t>Win Rate</t>
   </si>
   <si>
-    <t>Encounter Rate</t>
-  </si>
-  <si>
     <t>What are we checking for? (Win Rate)</t>
-  </si>
-  <si>
-    <t>(Encounter Rate)</t>
   </si>
   <si>
     <t>(Taken Rate)</t>
@@ -531,10 +525,10 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -542,10 +536,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -553,10 +547,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -564,10 +558,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -575,7 +569,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -588,7 +582,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -596,67 +590,67 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="F12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -666,10 +660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872B2F17-0633-4A96-A1FA-4F4EA4EC978C}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -679,7 +673,7 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -692,16 +686,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -723,7 +714,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -738,36 +729,6 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D19" t="s">
         <v>4</v>
       </c>
     </row>
@@ -788,13 +749,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -802,10 +763,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -813,10 +774,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -824,10 +785,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -835,7 +796,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -848,7 +809,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -856,62 +817,62 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -924,20 +885,20 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
@@ -945,10 +906,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
@@ -956,7 +917,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
@@ -964,7 +925,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
@@ -972,7 +933,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">

</xml_diff>